<commit_message>
update attendacne - can check if class study by session and day instead day as prev version. fix some bug at: home, cart. certificate,.. add preview file after uploaded by user in question detail and course detail
</commit_message>
<xml_diff>
--- a/f4education/backend/src/main/resources/static/excel/questionDetail.xlsx
+++ b/f4education/backend/src/main/resources/static/excel/questionDetail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HienTran\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA43885-4F13-4D5B-8703-AC73F84F4C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B095A2C-34E6-4774-B658-B9B8B371D1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>Answer Four</t>
   </si>
   <si>
-    <t>Nội dung câu hỏi</t>
-  </si>
-  <si>
     <t>Dùng eclipse</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Đúng/sai</t>
+  </si>
+  <si>
+    <t>Nội dung câu trả lời</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,21 +489,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>1</v>
@@ -511,10 +511,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>1</v>
@@ -522,10 +522,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>1</v>
@@ -533,10 +533,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>1</v>
@@ -544,10 +544,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="b">
         <v>1</v>
@@ -555,10 +555,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>1</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -588,10 +588,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>0</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="b">
         <v>0</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>0</v>
@@ -621,10 +621,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>1</v>
@@ -632,10 +632,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>1</v>
@@ -643,10 +643,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
@@ -654,10 +654,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>0</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>0</v>
@@ -676,10 +676,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C18" s="3" t="b">
         <v>1</v>
@@ -687,10 +687,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="3" t="b">
         <v>1</v>
@@ -698,10 +698,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>1</v>

</xml_diff>